<commit_message>
first draft of Gantt Chart (incomplete)
</commit_message>
<xml_diff>
--- a/figures&tables/Gantt Chart.xlsx
+++ b/figures&tables/Gantt Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalto\Documents\workspaces\Automatically-Generated-Cyber-Security-Compliance-Engine\figures&amp;tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EDC182B-04C2-4D8B-A029-F6459AE50AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1496C7-26E6-4166-BA97-72A80386652A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{BFC6B867-B639-4663-95F5-CA0E4A3138AF}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="18160" windowHeight="11560" xr2:uid="{BFC6B867-B639-4663-95F5-CA0E4A3138AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>October</t>
   </si>
@@ -63,39 +63,18 @@
     <t>Write up</t>
   </si>
   <si>
-    <t>Project Plan</t>
-  </si>
-  <si>
-    <t>Time allocation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Final Gantt Chart </t>
   </si>
   <si>
-    <t>Background Research</t>
-  </si>
-  <si>
-    <t>Follow up background research</t>
-  </si>
-  <si>
     <t>Literature review</t>
   </si>
   <si>
     <t>Design</t>
   </si>
   <si>
-    <t xml:space="preserve">Approach </t>
-  </si>
-  <si>
     <t>Progress report</t>
   </si>
   <si>
-    <t>Review of background literature</t>
-  </si>
-  <si>
-    <t>A clear statement of the problem and goals of the project</t>
-  </si>
-  <si>
     <t>An analysis and specification of the solution to the problem</t>
   </si>
   <si>
@@ -123,25 +102,40 @@
     <t>Project viva</t>
   </si>
   <si>
-    <t>Network set-up</t>
-  </si>
-  <si>
-    <t>Malware set-up</t>
-  </si>
-  <si>
-    <t>Tooling set-up</t>
-  </si>
-  <si>
     <t>Confirm analysis methods</t>
   </si>
   <si>
     <t>Final report</t>
   </si>
   <si>
-    <t>Investigation</t>
-  </si>
-  <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Planning diagrams (System overview, use-case, etc)</t>
+  </si>
+  <si>
+    <t>Robot Framework setup</t>
+  </si>
+  <si>
+    <t>Test implementation</t>
+  </si>
+  <si>
+    <t>Introduction, including: A clear statement of the problem and goals of the project</t>
+  </si>
+  <si>
+    <t>Viva</t>
+  </si>
+  <si>
+    <t>Time Management Planning</t>
+  </si>
+  <si>
+    <t>Further background research</t>
+  </si>
+  <si>
+    <t>Background research</t>
   </si>
 </sst>
 </file>
@@ -180,13 +174,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,9 +202,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -526,202 +520,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1EC7EB-9EFD-493A-8173-1DE58C5CC14D}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4"/>
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="2"/>
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2"/>
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
       <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="4"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="4"/>
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -729,87 +719,97 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1" t="s">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" s="1" t="s">
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="4"/>
-      <c r="B32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edited template and completed gantt chart
</commit_message>
<xml_diff>
--- a/figures&tables/Gantt Chart.xlsx
+++ b/figures&tables/Gantt Chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalto\Documents\workspaces\Automatically-Generated-Cyber-Security-Compliance-Engine\figures&amp;tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1496C7-26E6-4166-BA97-72A80386652A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{5D1496C7-26E6-4166-BA97-72A80386652A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{066F3DED-04F4-44C1-B99E-06C830F90C26}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="18160" windowHeight="11560" xr2:uid="{BFC6B867-B639-4663-95F5-CA0E4A3138AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>October</t>
   </si>
@@ -75,36 +75,9 @@
     <t>Progress report</t>
   </si>
   <si>
-    <t>An analysis and specification of the solution to the problem</t>
-  </si>
-  <si>
-    <t>A detailed design</t>
-  </si>
-  <si>
-    <t>The implementation</t>
-  </si>
-  <si>
-    <t>Testing strategy and results</t>
-  </si>
-  <si>
-    <t>A critical evaluation</t>
-  </si>
-  <si>
-    <t>Conclusions and future work</t>
-  </si>
-  <si>
-    <t>References to the literature</t>
-  </si>
-  <si>
-    <t>Appendices providing detailed technical references</t>
-  </si>
-  <si>
     <t>Project viva</t>
   </si>
   <si>
-    <t>Confirm analysis methods</t>
-  </si>
-  <si>
     <t>Final report</t>
   </si>
   <si>
@@ -136,23 +109,55 @@
   </si>
   <si>
     <t>Background research</t>
+  </si>
+  <si>
+    <t>Script to extract CSV data</t>
+  </si>
+  <si>
+    <t>Cloud application for managing accounts/forms</t>
+  </si>
+  <si>
+    <t>Form creation from CSV data</t>
+  </si>
+  <si>
+    <t>Designs</t>
+  </si>
+  <si>
+    <t>Results and Analysis</t>
+  </si>
+  <si>
+    <t>Testing and Software Validation</t>
+  </si>
+  <si>
+    <t>Background and Literature Review</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Conclusions</t>
+  </si>
+  <si>
+    <t>Future Work</t>
+  </si>
+  <si>
+    <t>Bibliography</t>
+  </si>
+  <si>
+    <t>Appendices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -193,19 +198,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF505050"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF505050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF505050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF505050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF505050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF505050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,296 +633,485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1EC7EB-9EFD-493A-8173-1DE58C5CC14D}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C34" sqref="C34:I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.43359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="E22" s="5"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="5"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="1" t="s">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-      <c r="B26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-      <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="4"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>